<commit_message>
Revisi laporan BA SO Tahap 2
</commit_message>
<xml_diff>
--- a/utility/optbs/template/berita_acara_stock_opname.xlsx
+++ b/utility/optbs/template/berita_acara_stock_opname.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>SKPD</t>
   </si>
@@ -46,7 +46,7 @@
     <t>STOCK OPNAME PERSEDIAAN</t>
   </si>
   <si>
-    <t>SEMESTER : </t>
+    <t>SEMESTER : [c.semester]</t>
   </si>
   <si>
     <t>NO</t>
@@ -127,7 +127,7 @@
     <t>[a.total_harga_saldo_awal;ope=tbs:num]</t>
   </si>
   <si>
-    <t> [a.subtotal_saldo_awal; block=row; when [a.cetak_subtotal]=1]</t>
+    <t> [a.counter; block=row; when [a.cetak_subtotal]=1]</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -151,7 +151,13 @@
     <t>Kota Pekalongan, [b.tanggal_cetak]</t>
   </si>
   <si>
-    <t>An Pengguna / Kuasa Pengguna Barang Pengurus Barang Pembantu Pengurus Barang</t>
+    <t>An Pengguna / Kuasa Pengguna Barang </t>
+  </si>
+  <si>
+    <t>Pengurus Barang </t>
+  </si>
+  <si>
+    <t>Pembantu Pengurus Barang</t>
   </si>
   <si>
     <t>Pejabat Penatausahaan Pengguna Barang</t>
@@ -569,16 +575,16 @@
   </sheetPr>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.24223602484472"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.3726708074534"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.5962732919255"/>
-    <col collapsed="false" hidden="false" max="15" min="4" style="0" width="17.7515527950311"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.360248447205"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8695652173913"/>
+    <col collapsed="false" hidden="false" max="15" min="4" style="0" width="18.4037267080745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,17 +970,21 @@
       </c>
       <c r="B18" s="34"/>
       <c r="E18" s="34"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="34"/>
-      <c r="L18" s="1"/>
+      <c r="L18" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="M18" s="37"/>
       <c r="N18" s="38"/>
     </row>
     <row r="19" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B19" s="34"/>
       <c r="E19" s="34"/>
@@ -1021,39 +1031,39 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="41" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="42"/>
       <c r="D24" s="43"/>
       <c r="E24" s="42"/>
       <c r="F24" s="41" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G24" s="41"/>
       <c r="H24" s="41"/>
       <c r="I24" s="42"/>
       <c r="L24" s="41" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M24" s="39"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
       <c r="D25" s="45"/>
       <c r="E25" s="44"/>
       <c r="F25" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="44"/>
       <c r="L25" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M25" s="39"/>
     </row>

</xml_diff>

<commit_message>
Revisi laporan stock opname
</commit_message>
<xml_diff>
--- a/utility/optbs/template/berita_acara_stock_opname.xlsx
+++ b/utility/optbs/template/berita_acara_stock_opname.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>SKPD</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>[a.subtotal_masuk; ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.subtotal_keluar; ope=tbs:num]</t>
   </si>
   <si>
     <t>[a.subtotal_sisa; ope=tbs:num]</t>
@@ -576,15 +579,15 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.24223602484472"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.360248447205"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8695652173913"/>
-    <col collapsed="false" hidden="false" max="15" min="4" style="0" width="18.4037267080745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.3478260869565"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.5155279503106"/>
+    <col collapsed="false" hidden="false" max="15" min="4" style="0" width="18.9006211180124"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,18 +906,20 @@
       </c>
       <c r="J14" s="24"/>
       <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
+      <c r="L14" s="24" t="s">
+        <v>39</v>
+      </c>
       <c r="M14" s="24"/>
       <c r="N14" s="24"/>
       <c r="O14" s="24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="30.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="25"/>
       <c r="B15" s="20"/>
       <c r="C15" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="27"/>
@@ -948,7 +953,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="33" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="33"/>
@@ -960,31 +965,31 @@
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
       <c r="L17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M17" s="36"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="34" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B18" s="34"/>
       <c r="E18" s="34"/>
       <c r="F18" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="34"/>
       <c r="L18" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M18" s="37"/>
       <c r="N18" s="38"/>
     </row>
     <row r="19" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B19" s="34"/>
       <c r="E19" s="34"/>
@@ -1031,39 +1036,39 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="42"/>
       <c r="D24" s="43"/>
       <c r="E24" s="42"/>
       <c r="F24" s="41" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G24" s="41"/>
       <c r="H24" s="41"/>
       <c r="I24" s="42"/>
       <c r="L24" s="41" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M24" s="39"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
       <c r="D25" s="45"/>
       <c r="E25" s="44"/>
       <c r="F25" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="44"/>
       <c r="L25" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M25" s="39"/>
     </row>

</xml_diff>

<commit_message>
Fix Grand Total Stock Opname
</commit_message>
<xml_diff>
--- a/utility/optbs/template/berita_acara_stock_opname.xlsx
+++ b/utility/optbs/template/berita_acara_stock_opname.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>SKPD</t>
   </si>
@@ -143,6 +143,15 @@
   </si>
   <si>
     <t>GRAND TOTAL</t>
+  </si>
+  <si>
+    <t>[d.grandTotal_saldoAwal; ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[d.grandTotal_penerimaan; ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[d.grandTotal_pengeluaran; ope=tbs:num]</t>
   </si>
   <si>
     <t>Mengetahui</t>
@@ -335,7 +344,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -424,6 +433,10 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -448,7 +461,7 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -466,6 +479,22 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -529,19 +558,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:AN25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O14" activeCellId="7" sqref="D13 E13:F14 G12:I12 H14:I14 J12:J13 K12:L14 M12:O13 O14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15:AN15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.24223602484472"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.472049689441"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.4844720496894"/>
-    <col collapsed="false" hidden="false" max="15" min="4" style="1" width="20.3788819875776"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="9.20496894409938"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.0869565217391"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.7888198757764"/>
+    <col collapsed="false" hidden="false" max="15" min="4" style="1" width="22.0186335403727"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="9.69565217391304"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,216 +913,250 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="30.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23" t="s">
+      <c r="B14" s="23"/>
+      <c r="C14" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26" t="s">
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="27"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26" t="s">
+      <c r="G14" s="28"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="27"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26" t="s">
+      <c r="J14" s="28"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="28" t="e">
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="29" t="e">
         <f aca="true">INDIRECT( "F" &amp; ROW() )+INDIRECT( "I" &amp; ROW() )-INDIRECT( "L" &amp; ROW() )</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="30.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23" t="s">
+      <c r="A15" s="30"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="33"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="36"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M15" s="36"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26" t="e">
+        <f aca="true">INDIRECT( "F" &amp; ROW() )+INDIRECT( "I" &amp; ROW() )-INDIRECT( "L" &amp; ROW() )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="37"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="37"/>
+      <c r="Z15" s="37"/>
+      <c r="AA15" s="37"/>
+      <c r="AB15" s="37"/>
+      <c r="AC15" s="37"/>
+      <c r="AD15" s="37"/>
+      <c r="AE15" s="37"/>
+      <c r="AF15" s="37"/>
+      <c r="AG15" s="37"/>
+      <c r="AH15" s="37"/>
+      <c r="AI15" s="37"/>
+      <c r="AJ15" s="37"/>
+      <c r="AK15" s="37"/>
+      <c r="AL15" s="37"/>
+      <c r="AM15" s="37"/>
+      <c r="AN15" s="37"/>
     </row>
     <row r="16" customFormat="false" ht="30.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="0"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
       <c r="G16" s="0"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
       <c r="J16" s="0"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
       <c r="M16" s="0"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="A17" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
       <c r="L17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M17" s="35"/>
+        <v>45</v>
+      </c>
+      <c r="M17" s="40"/>
       <c r="N17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="36"/>
+      <c r="A18" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="41"/>
       <c r="C18" s="0"/>
       <c r="D18" s="0"/>
-      <c r="E18" s="36"/>
+      <c r="E18" s="41"/>
       <c r="F18" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="36"/>
+      <c r="I18" s="41"/>
       <c r="L18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
+        <v>48</v>
+      </c>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
     </row>
     <row r="19" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="36"/>
+        <v>49</v>
+      </c>
+      <c r="B19" s="41"/>
       <c r="C19" s="0"/>
       <c r="D19" s="0"/>
-      <c r="E19" s="36"/>
+      <c r="E19" s="41"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="36"/>
+      <c r="I19" s="41"/>
       <c r="L19" s="2"/>
       <c r="M19" s="0"/>
       <c r="N19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="38"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="0"/>
       <c r="C20" s="0"/>
       <c r="D20" s="0"/>
       <c r="E20" s="0"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
       <c r="I20" s="0"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="38"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
       <c r="D21" s="0"/>
       <c r="E21" s="0"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
       <c r="I21" s="0"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="42"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="38"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="0"/>
       <c r="C22" s="0"/>
       <c r="D22" s="0"/>
       <c r="E22" s="0"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
       <c r="I22" s="0"/>
-      <c r="L22" s="38"/>
+      <c r="L22" s="43"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="38"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
       <c r="D23" s="0"/>
       <c r="E23" s="0"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
       <c r="I23" s="0"/>
-      <c r="L23" s="38"/>
+      <c r="L23" s="43"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="40"/>
-      <c r="L24" s="39" t="s">
-        <v>49</v>
+      <c r="A24" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="45"/>
+      <c r="L24" s="44" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="42"/>
+        <v>53</v>
+      </c>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="47"/>
       <c r="F25" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="42"/>
+      <c r="I25" s="47"/>
       <c r="L25" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="16">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="A2:B2"/>
@@ -1110,12 +1173,10 @@
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="M9:O9"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.590277777777778" right="1.575" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="5" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.6" right="0.820138888888889" top="0.6" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Fix Report BA Stock Opname
</commit_message>
<xml_diff>
--- a/utility/optbs/template/berita_acara_stock_opname.xlsx
+++ b/utility/optbs/template/berita_acara_stock_opname.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>SKPD</t>
   </si>
@@ -46,7 +46,7 @@
     <t>STOCK OPNAME PERSEDIAAN</t>
   </si>
   <si>
-    <t>SEMESTER : [c.semester]</t>
+    <t>PER TANGGAL : [c.tanggal]</t>
   </si>
   <si>
     <t>NO</t>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>An Pengguna / Kuasa Pengguna Barang </t>
-  </si>
-  <si>
-    <t>Pengurus Barang </t>
   </si>
   <si>
     <t>Pembantu Pengurus Barang</t>
@@ -560,17 +557,17 @@
   </sheetPr>
   <dimension ref="A1:AN25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15:AN15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.24223602484472"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.0869565217391"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.7888198757764"/>
-    <col collapsed="false" hidden="false" max="15" min="4" style="1" width="22.0186335403727"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="9.69565217391304"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.8633540372671"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.416149068323"/>
+    <col collapsed="false" hidden="false" max="15" min="4" style="1" width="23.9937888198758"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="10.1863354037267"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,6 +590,31 @@
       <c r="M1" s="0"/>
       <c r="N1" s="0"/>
       <c r="O1" s="0"/>
+      <c r="P1" s="0"/>
+      <c r="Q1" s="0"/>
+      <c r="R1" s="0"/>
+      <c r="S1" s="0"/>
+      <c r="T1" s="0"/>
+      <c r="U1" s="0"/>
+      <c r="V1" s="0"/>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
+      <c r="AA1" s="0"/>
+      <c r="AB1" s="0"/>
+      <c r="AC1" s="0"/>
+      <c r="AD1" s="0"/>
+      <c r="AE1" s="0"/>
+      <c r="AF1" s="0"/>
+      <c r="AG1" s="0"/>
+      <c r="AH1" s="0"/>
+      <c r="AI1" s="0"/>
+      <c r="AJ1" s="0"/>
+      <c r="AK1" s="0"/>
+      <c r="AL1" s="0"/>
+      <c r="AM1" s="0"/>
+      <c r="AN1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -614,6 +636,31 @@
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
       <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
+      <c r="AJ2" s="0"/>
+      <c r="AK2" s="0"/>
+      <c r="AL2" s="0"/>
+      <c r="AM2" s="0"/>
+      <c r="AN2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -635,6 +682,31 @@
       <c r="M3" s="0"/>
       <c r="N3" s="0"/>
       <c r="O3" s="0"/>
+      <c r="P3" s="0"/>
+      <c r="Q3" s="0"/>
+      <c r="R3" s="0"/>
+      <c r="S3" s="0"/>
+      <c r="T3" s="0"/>
+      <c r="U3" s="0"/>
+      <c r="V3" s="0"/>
+      <c r="W3" s="0"/>
+      <c r="X3" s="0"/>
+      <c r="Y3" s="0"/>
+      <c r="Z3" s="0"/>
+      <c r="AA3" s="0"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="0"/>
+      <c r="AD3" s="0"/>
+      <c r="AE3" s="0"/>
+      <c r="AF3" s="0"/>
+      <c r="AG3" s="0"/>
+      <c r="AH3" s="0"/>
+      <c r="AI3" s="0"/>
+      <c r="AJ3" s="0"/>
+      <c r="AK3" s="0"/>
+      <c r="AL3" s="0"/>
+      <c r="AM3" s="0"/>
+      <c r="AN3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
@@ -652,6 +724,31 @@
       <c r="M4" s="0"/>
       <c r="N4" s="0"/>
       <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
+      <c r="X4" s="0"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="0"/>
+      <c r="AA4" s="0"/>
+      <c r="AB4" s="0"/>
+      <c r="AC4" s="0"/>
+      <c r="AD4" s="0"/>
+      <c r="AE4" s="0"/>
+      <c r="AF4" s="0"/>
+      <c r="AG4" s="0"/>
+      <c r="AH4" s="0"/>
+      <c r="AI4" s="0"/>
+      <c r="AJ4" s="0"/>
+      <c r="AK4" s="0"/>
+      <c r="AL4" s="0"/>
+      <c r="AM4" s="0"/>
+      <c r="AN4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
@@ -671,6 +768,31 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
+      <c r="P5" s="0"/>
+      <c r="Q5" s="0"/>
+      <c r="R5" s="0"/>
+      <c r="S5" s="0"/>
+      <c r="T5" s="0"/>
+      <c r="U5" s="0"/>
+      <c r="V5" s="0"/>
+      <c r="W5" s="0"/>
+      <c r="X5" s="0"/>
+      <c r="Y5" s="0"/>
+      <c r="Z5" s="0"/>
+      <c r="AA5" s="0"/>
+      <c r="AB5" s="0"/>
+      <c r="AC5" s="0"/>
+      <c r="AD5" s="0"/>
+      <c r="AE5" s="0"/>
+      <c r="AF5" s="0"/>
+      <c r="AG5" s="0"/>
+      <c r="AH5" s="0"/>
+      <c r="AI5" s="0"/>
+      <c r="AJ5" s="0"/>
+      <c r="AK5" s="0"/>
+      <c r="AL5" s="0"/>
+      <c r="AM5" s="0"/>
+      <c r="AN5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -690,6 +812,31 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
+      <c r="P6" s="0"/>
+      <c r="Q6" s="0"/>
+      <c r="R6" s="0"/>
+      <c r="S6" s="0"/>
+      <c r="T6" s="0"/>
+      <c r="U6" s="0"/>
+      <c r="V6" s="0"/>
+      <c r="W6" s="0"/>
+      <c r="X6" s="0"/>
+      <c r="Y6" s="0"/>
+      <c r="Z6" s="0"/>
+      <c r="AA6" s="0"/>
+      <c r="AB6" s="0"/>
+      <c r="AC6" s="0"/>
+      <c r="AD6" s="0"/>
+      <c r="AE6" s="0"/>
+      <c r="AF6" s="0"/>
+      <c r="AG6" s="0"/>
+      <c r="AH6" s="0"/>
+      <c r="AI6" s="0"/>
+      <c r="AJ6" s="0"/>
+      <c r="AK6" s="0"/>
+      <c r="AL6" s="0"/>
+      <c r="AM6" s="0"/>
+      <c r="AN6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
@@ -709,6 +856,31 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="0"/>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+      <c r="V7" s="0"/>
+      <c r="W7" s="0"/>
+      <c r="X7" s="0"/>
+      <c r="Y7" s="0"/>
+      <c r="Z7" s="0"/>
+      <c r="AA7" s="0"/>
+      <c r="AB7" s="0"/>
+      <c r="AC7" s="0"/>
+      <c r="AD7" s="0"/>
+      <c r="AE7" s="0"/>
+      <c r="AF7" s="0"/>
+      <c r="AG7" s="0"/>
+      <c r="AH7" s="0"/>
+      <c r="AI7" s="0"/>
+      <c r="AJ7" s="0"/>
+      <c r="AK7" s="0"/>
+      <c r="AL7" s="0"/>
+      <c r="AM7" s="0"/>
+      <c r="AN7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0"/>
@@ -726,6 +898,31 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="0"/>
+      <c r="P8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
+      <c r="S8" s="0"/>
+      <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+      <c r="V8" s="0"/>
+      <c r="W8" s="0"/>
+      <c r="X8" s="0"/>
+      <c r="Y8" s="0"/>
+      <c r="Z8" s="0"/>
+      <c r="AA8" s="0"/>
+      <c r="AB8" s="0"/>
+      <c r="AC8" s="0"/>
+      <c r="AD8" s="0"/>
+      <c r="AE8" s="0"/>
+      <c r="AF8" s="0"/>
+      <c r="AG8" s="0"/>
+      <c r="AH8" s="0"/>
+      <c r="AI8" s="0"/>
+      <c r="AJ8" s="0"/>
+      <c r="AK8" s="0"/>
+      <c r="AL8" s="0"/>
+      <c r="AM8" s="0"/>
+      <c r="AN8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="27.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
@@ -757,6 +954,31 @@
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
+      <c r="P9" s="0"/>
+      <c r="Q9" s="0"/>
+      <c r="R9" s="0"/>
+      <c r="S9" s="0"/>
+      <c r="T9" s="0"/>
+      <c r="U9" s="0"/>
+      <c r="V9" s="0"/>
+      <c r="W9" s="0"/>
+      <c r="X9" s="0"/>
+      <c r="Y9" s="0"/>
+      <c r="Z9" s="0"/>
+      <c r="AA9" s="0"/>
+      <c r="AB9" s="0"/>
+      <c r="AC9" s="0"/>
+      <c r="AD9" s="0"/>
+      <c r="AE9" s="0"/>
+      <c r="AF9" s="0"/>
+      <c r="AG9" s="0"/>
+      <c r="AH9" s="0"/>
+      <c r="AI9" s="0"/>
+      <c r="AJ9" s="0"/>
+      <c r="AK9" s="0"/>
+      <c r="AL9" s="0"/>
+      <c r="AM9" s="0"/>
+      <c r="AN9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="30.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6"/>
@@ -798,6 +1020,31 @@
       <c r="O10" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="P10" s="0"/>
+      <c r="Q10" s="0"/>
+      <c r="R10" s="0"/>
+      <c r="S10" s="0"/>
+      <c r="T10" s="0"/>
+      <c r="U10" s="0"/>
+      <c r="V10" s="0"/>
+      <c r="W10" s="0"/>
+      <c r="X10" s="0"/>
+      <c r="Y10" s="0"/>
+      <c r="Z10" s="0"/>
+      <c r="AA10" s="0"/>
+      <c r="AB10" s="0"/>
+      <c r="AC10" s="0"/>
+      <c r="AD10" s="0"/>
+      <c r="AE10" s="0"/>
+      <c r="AF10" s="0"/>
+      <c r="AG10" s="0"/>
+      <c r="AH10" s="0"/>
+      <c r="AI10" s="0"/>
+      <c r="AJ10" s="0"/>
+      <c r="AK10" s="0"/>
+      <c r="AL10" s="0"/>
+      <c r="AM10" s="0"/>
+      <c r="AN10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="30.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
@@ -817,6 +1064,31 @@
       <c r="M11" s="13"/>
       <c r="N11" s="14"/>
       <c r="O11" s="15"/>
+      <c r="P11" s="0"/>
+      <c r="Q11" s="0"/>
+      <c r="R11" s="0"/>
+      <c r="S11" s="0"/>
+      <c r="T11" s="0"/>
+      <c r="U11" s="0"/>
+      <c r="V11" s="0"/>
+      <c r="W11" s="0"/>
+      <c r="X11" s="0"/>
+      <c r="Y11" s="0"/>
+      <c r="Z11" s="0"/>
+      <c r="AA11" s="0"/>
+      <c r="AB11" s="0"/>
+      <c r="AC11" s="0"/>
+      <c r="AD11" s="0"/>
+      <c r="AE11" s="0"/>
+      <c r="AF11" s="0"/>
+      <c r="AG11" s="0"/>
+      <c r="AH11" s="0"/>
+      <c r="AI11" s="0"/>
+      <c r="AJ11" s="0"/>
+      <c r="AK11" s="0"/>
+      <c r="AL11" s="0"/>
+      <c r="AM11" s="0"/>
+      <c r="AN11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="30.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
@@ -864,6 +1136,31 @@
       <c r="O12" s="21" t="s">
         <v>30</v>
       </c>
+      <c r="P12" s="0"/>
+      <c r="Q12" s="0"/>
+      <c r="R12" s="0"/>
+      <c r="S12" s="0"/>
+      <c r="T12" s="0"/>
+      <c r="U12" s="0"/>
+      <c r="V12" s="0"/>
+      <c r="W12" s="0"/>
+      <c r="X12" s="0"/>
+      <c r="Y12" s="0"/>
+      <c r="Z12" s="0"/>
+      <c r="AA12" s="0"/>
+      <c r="AB12" s="0"/>
+      <c r="AC12" s="0"/>
+      <c r="AD12" s="0"/>
+      <c r="AE12" s="0"/>
+      <c r="AF12" s="0"/>
+      <c r="AG12" s="0"/>
+      <c r="AH12" s="0"/>
+      <c r="AI12" s="0"/>
+      <c r="AJ12" s="0"/>
+      <c r="AK12" s="0"/>
+      <c r="AL12" s="0"/>
+      <c r="AM12" s="0"/>
+      <c r="AN12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="30.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
@@ -911,6 +1208,31 @@
       <c r="O13" s="21" t="s">
         <v>30</v>
       </c>
+      <c r="P13" s="0"/>
+      <c r="Q13" s="0"/>
+      <c r="R13" s="0"/>
+      <c r="S13" s="0"/>
+      <c r="T13" s="0"/>
+      <c r="U13" s="0"/>
+      <c r="V13" s="0"/>
+      <c r="W13" s="0"/>
+      <c r="X13" s="0"/>
+      <c r="Y13" s="0"/>
+      <c r="Z13" s="0"/>
+      <c r="AA13" s="0"/>
+      <c r="AB13" s="0"/>
+      <c r="AC13" s="0"/>
+      <c r="AD13" s="0"/>
+      <c r="AE13" s="0"/>
+      <c r="AF13" s="0"/>
+      <c r="AG13" s="0"/>
+      <c r="AH13" s="0"/>
+      <c r="AI13" s="0"/>
+      <c r="AJ13" s="0"/>
+      <c r="AK13" s="0"/>
+      <c r="AL13" s="0"/>
+      <c r="AM13" s="0"/>
+      <c r="AN13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="30.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
@@ -941,6 +1263,31 @@
         <f aca="true">INDIRECT( "F" &amp; ROW() )+INDIRECT( "I" &amp; ROW() )-INDIRECT( "L" &amp; ROW() )</f>
         <v>#VALUE!</v>
       </c>
+      <c r="P14" s="0"/>
+      <c r="Q14" s="0"/>
+      <c r="R14" s="0"/>
+      <c r="S14" s="0"/>
+      <c r="T14" s="0"/>
+      <c r="U14" s="0"/>
+      <c r="V14" s="0"/>
+      <c r="W14" s="0"/>
+      <c r="X14" s="0"/>
+      <c r="Y14" s="0"/>
+      <c r="Z14" s="0"/>
+      <c r="AA14" s="0"/>
+      <c r="AB14" s="0"/>
+      <c r="AC14" s="0"/>
+      <c r="AD14" s="0"/>
+      <c r="AE14" s="0"/>
+      <c r="AF14" s="0"/>
+      <c r="AG14" s="0"/>
+      <c r="AH14" s="0"/>
+      <c r="AI14" s="0"/>
+      <c r="AJ14" s="0"/>
+      <c r="AK14" s="0"/>
+      <c r="AL14" s="0"/>
+      <c r="AM14" s="0"/>
+      <c r="AN14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="30.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="30"/>
@@ -1039,21 +1386,19 @@
       <c r="C18" s="0"/>
       <c r="D18" s="0"/>
       <c r="E18" s="41"/>
-      <c r="F18" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="41"/>
       <c r="L18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M18" s="42"/>
       <c r="N18" s="42"/>
     </row>
     <row r="19" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="41"/>
       <c r="C19" s="0"/>
@@ -1121,38 +1466,38 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="45"/>
       <c r="C24" s="45"/>
       <c r="D24" s="46"/>
       <c r="E24" s="45"/>
       <c r="F24" s="44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
       <c r="I24" s="45"/>
       <c r="L24" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="47"/>
       <c r="C25" s="47"/>
       <c r="D25" s="48"/>
       <c r="E25" s="47"/>
       <c r="F25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="47"/>
       <c r="L25" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>